<commit_message>
Insertando Contenido de un excel
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexandra.veizu\Documents\Reframework_update_UiPath_Services\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jperezm2\OneDrive - Capgemini\Documents\UiPath\RoboticEnterpriseFramework\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BE7DFF5-5AFC-4110-8461-609B0BDD5551}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C96E53EC-3B1A-4CE2-AEF8-B94114DF6D1F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
   <si>
     <t>Name</t>
   </si>
@@ -122,6 +122,12 @@
   </si>
   <si>
     <t>OrchestratorAssetFolder</t>
+  </si>
+  <si>
+    <t>PathDocuments</t>
+  </si>
+  <si>
+    <t>C:\Users\jperezm2\Downloads\</t>
   </si>
 </sst>
 </file>
@@ -499,16 +505,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5703125" customWidth="1"/>
+    <col min="1" max="1" width="43.54296875" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="81.453125" customWidth="1"/>
+    <col min="4" max="26" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -557,7 +563,7 @@
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="4" spans="1:26" ht="30">
+    <row r="4" spans="1:26" ht="29">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -568,7 +574,14 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" t="s">
+        <v>33</v>
+      </c>
+    </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1574,12 +1587,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="75.453125" customWidth="1"/>
+    <col min="4" max="26" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1616,7 +1629,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="30">
+    <row r="2" spans="1:26" ht="29">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2682,16 +2695,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="A2:C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" customWidth="1"/>
-    <col min="2" max="2" width="30.140625" customWidth="1"/>
-    <col min="3" max="3" width="60.28515625" customWidth="1"/>
-    <col min="4" max="26" width="65.42578125" customWidth="1"/>
+    <col min="1" max="1" width="31.81640625" customWidth="1"/>
+    <col min="2" max="2" width="30.1796875" customWidth="1"/>
+    <col min="3" max="3" width="60.26953125" customWidth="1"/>
+    <col min="4" max="26" width="65.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>